<commit_message>
INFO and tasks A1-A6
</commit_message>
<xml_diff>
--- a/Kutuzov17/evidence.xlsx
+++ b/Kutuzov17/evidence.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="43">
   <si>
     <t>TxHash</t>
   </si>
@@ -78,24 +78,6 @@
     <t>nft id</t>
   </si>
   <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
-  </si>
-  <si>
-    <t>nft id you minted</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -142,6 +124,54 @@
   </si>
   <si>
     <t>uptick1xwjqw7upd43d3u2ntjsxs3vx0ppr7f68dp75gy</t>
+  </si>
+  <si>
+    <t>5BE98606491C22D11BE5DD582E2C73A565045352CDB24B42D977917A10EF43AA</t>
+  </si>
+  <si>
+    <t>kutuzovGoNFT</t>
+  </si>
+  <si>
+    <t>DF82067D3F012AC718B305C0BC16359549FE277D5F190FBD03682D2F52E1A942</t>
+  </si>
+  <si>
+    <t>kutuzov001</t>
+  </si>
+  <si>
+    <t>0C0BC912BB7B3E36AA048B951DCD273654BD0CE21978B86B4A13218615D018B1</t>
+  </si>
+  <si>
+    <t>kutuzov002</t>
+  </si>
+  <si>
+    <t>B51980F0DB66DE20ED132647BA95D76259F7759108DC02480E6038C4293AAE41</t>
+  </si>
+  <si>
+    <t>kutuzov003</t>
+  </si>
+  <si>
+    <t>3FC7A59A824783A62274AEA5F2E73E3E1417421B5986B3850BD83F17CBC66829</t>
+  </si>
+  <si>
+    <t>wasm.juno1ummdfdvtvs3wrnfntdz8tewceyp27ahledcz9qxzevkng8us45sss9dgg8</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>5569DA184716CACE8FA9E83DFFE31B1D31D170DE9BBEE49793E8E4EE159859E0</t>
+  </si>
+  <si>
+    <t>ibc/D3F28BB155F492C517E9ADD9044C85A94DDD54F3518557473CCA5C35696B6C8C</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>703384E75533522BCC1EC22247D4982A82A810574548E1FC28C7284E4A25C7E5</t>
+  </si>
+  <si>
+    <t>9DCED4F73F30CB88865F90E236205FD65F4B033A756FFBD52BCE8C7D5601EBBD</t>
   </si>
 </sst>
 </file>
@@ -550,7 +580,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,54 +597,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1072,7 +1102,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,12 +1118,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1339,10 +1369,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,15 +1392,37 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1386,7 +1438,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1409,18 +1463,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1436,7 +1490,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1460,18 +1514,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1488,7 +1542,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,18 +1566,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1540,7 +1594,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,18 +1619,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>